<commit_message>
Codigo Capitulo 8 parte 2
</commit_message>
<xml_diff>
--- a/Codigos/Cap8/VHDLCAP8.xlsx
+++ b/Codigos/Cap8/VHDLCAP8.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Planilha1 (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="65">
   <si>
     <t>*</t>
   </si>
@@ -215,13 +214,19 @@
   </si>
   <si>
     <t>548D</t>
+  </si>
+  <si>
+    <t>Y (decimal)</t>
+  </si>
+  <si>
+    <t>Y (binário)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +253,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -825,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1109,21 +1121,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1145,6 +1142,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1660,53 +1682,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="P60" sqref="P60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1715,113 +1739,157 @@
       </c>
       <c r="H8" s="104"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="H9" s="104"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
       <c r="H10" s="104"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
       <c r="H11" s="104"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
-      <c r="H12" s="104"/>
-      <c r="O12" s="5">
+      <c r="D12" s="104" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="104"/>
+      <c r="H12" s="126" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="126" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="126" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="126" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="126" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="126" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" s="5">
         <v>3</v>
       </c>
-      <c r="P12" s="5">
+      <c r="Q12" s="5">
         <v>2</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="R12" s="5">
         <v>1</v>
       </c>
-      <c r="R12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
-      <c r="E13" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="104"/>
-      <c r="N13" s="5" t="s">
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="104"/>
+      <c r="H13" s="125">
+        <v>1</v>
+      </c>
+      <c r="I13" s="125">
+        <v>0</v>
+      </c>
+      <c r="J13" s="125">
+        <v>0</v>
+      </c>
+      <c r="K13" s="125">
+        <v>0</v>
+      </c>
+      <c r="L13" s="125">
+        <f>36*H13+44*I13+164*J13+548*K13+36</f>
+        <v>72</v>
+      </c>
+      <c r="M13" s="125" t="str">
+        <f>DEC2BIN(INT(L13/512))&amp;DEC2BIN(MOD(L13,512),9)</f>
+        <v>0001001000</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="104"/>
-      <c r="N14" s="5" t="s">
+      <c r="G14" s="104"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="128"/>
+      <c r="M14" s="128"/>
+      <c r="O14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
       <c r="H15" s="104"/>
-      <c r="N15" s="5" t="s">
+      <c r="O15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
       <c r="H16" s="104"/>
-      <c r="N16" s="5" t="s">
+      <c r="O16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="Q16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1881,7 +1949,7 @@
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
-      <c r="D20" s="113" t="s">
+      <c r="D20" s="120" t="s">
         <v>59</v>
       </c>
       <c r="E20" s="105"/>
@@ -1915,7 +1983,7 @@
     </row>
     <row r="21" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="10"/>
-      <c r="D21" s="114"/>
+      <c r="D21" s="121"/>
       <c r="E21" s="106"/>
       <c r="F21" s="106"/>
       <c r="G21" s="106"/>
@@ -1935,7 +2003,7 @@
     </row>
     <row r="22" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
-      <c r="D22" s="115" t="s">
+      <c r="D22" s="122" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="107"/>
@@ -1969,7 +2037,7 @@
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
-      <c r="D23" s="116"/>
+      <c r="D23" s="123"/>
       <c r="E23" s="105"/>
       <c r="F23" s="105"/>
       <c r="G23" s="105"/>
@@ -1995,7 +2063,7 @@
     </row>
     <row r="24" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="10"/>
-      <c r="D24" s="114"/>
+      <c r="D24" s="121"/>
       <c r="E24" s="106"/>
       <c r="F24" s="106"/>
       <c r="G24" s="106"/>
@@ -2015,7 +2083,7 @@
     </row>
     <row r="25" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C25" s="10"/>
-      <c r="D25" s="115" t="s">
+      <c r="D25" s="122" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="107"/>
@@ -2053,7 +2121,7 @@
     </row>
     <row r="26" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="10"/>
-      <c r="D26" s="114"/>
+      <c r="D26" s="121"/>
       <c r="E26" s="106"/>
       <c r="F26" s="106"/>
       <c r="G26" s="106"/>
@@ -2077,7 +2145,7 @@
     </row>
     <row r="27" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C27" s="10"/>
-      <c r="D27" s="115" t="s">
+      <c r="D27" s="122" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="107"/>
@@ -2119,7 +2187,7 @@
     </row>
     <row r="28" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="10"/>
-      <c r="D28" s="114"/>
+      <c r="D28" s="121"/>
       <c r="E28" s="106"/>
       <c r="F28" s="106"/>
       <c r="G28" s="106"/>
@@ -2289,7 +2357,7 @@
     </row>
     <row r="35" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C35" s="10"/>
-      <c r="D35" s="120" t="s">
+      <c r="D35" s="115" t="s">
         <v>36</v>
       </c>
       <c r="E35" s="99"/>
@@ -2334,7 +2402,7 @@
     </row>
     <row r="36" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C36" s="10"/>
-      <c r="D36" s="121"/>
+      <c r="D36" s="116"/>
       <c r="E36" s="101"/>
       <c r="F36" s="101"/>
       <c r="G36" s="100"/>
@@ -2373,7 +2441,7 @@
     </row>
     <row r="37" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C37" s="10"/>
-      <c r="D37" s="121"/>
+      <c r="D37" s="116"/>
       <c r="E37" s="101"/>
       <c r="F37" s="101"/>
       <c r="G37" s="101"/>
@@ -2408,7 +2476,7 @@
     </row>
     <row r="38" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C38" s="10"/>
-      <c r="D38" s="121"/>
+      <c r="D38" s="116"/>
       <c r="E38" s="101"/>
       <c r="F38" s="101"/>
       <c r="G38" s="101"/>
@@ -2443,7 +2511,7 @@
     </row>
     <row r="39" spans="3:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C39" s="10"/>
-      <c r="D39" s="121"/>
+      <c r="D39" s="116"/>
       <c r="E39" s="101"/>
       <c r="F39" s="101"/>
       <c r="G39" s="101"/>
@@ -2478,7 +2546,7 @@
     </row>
     <row r="40" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C40" s="10"/>
-      <c r="D40" s="121"/>
+      <c r="D40" s="116"/>
       <c r="E40" s="101"/>
       <c r="F40" s="101"/>
       <c r="G40" s="101"/>
@@ -2505,7 +2573,7 @@
     </row>
     <row r="41" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C41" s="10"/>
-      <c r="D41" s="121"/>
+      <c r="D41" s="116"/>
       <c r="E41" s="101"/>
       <c r="F41" s="101"/>
       <c r="G41" s="101"/>
@@ -2532,7 +2600,7 @@
     </row>
     <row r="42" spans="3:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C42" s="10"/>
-      <c r="D42" s="122"/>
+      <c r="D42" s="117"/>
       <c r="E42" s="101"/>
       <c r="F42" s="101"/>
       <c r="G42" s="101"/>
@@ -2632,7 +2700,7 @@
       </c>
     </row>
     <row r="53" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="123" t="s">
+      <c r="D53" s="118" t="s">
         <v>5</v>
       </c>
       <c r="E53" s="1"/>
@@ -2679,7 +2747,7 @@
       </c>
     </row>
     <row r="54" spans="3:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="123"/>
+      <c r="D54" s="118"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="3"/>
@@ -2720,7 +2788,7 @@
       </c>
     </row>
     <row r="55" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D55" s="123"/>
+      <c r="D55" s="118"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -2757,7 +2825,7 @@
       </c>
     </row>
     <row r="56" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D56" s="123"/>
+      <c r="D56" s="118"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2794,7 +2862,7 @@
       </c>
     </row>
     <row r="57" spans="3:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D57" s="123"/>
+      <c r="D57" s="118"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2831,7 +2899,7 @@
       </c>
     </row>
     <row r="58" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D58" s="123"/>
+      <c r="D58" s="118"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -2860,7 +2928,7 @@
       </c>
     </row>
     <row r="59" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D59" s="123"/>
+      <c r="D59" s="118"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -2886,7 +2954,7 @@
       </c>
     </row>
     <row r="60" spans="3:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D60" s="123"/>
+      <c r="D60" s="118"/>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
@@ -2912,7 +2980,7 @@
       </c>
     </row>
     <row r="61" spans="3:21" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D61" s="118" t="s">
+      <c r="D61" s="113" t="s">
         <v>17</v>
       </c>
       <c r="E61" s="11"/>
@@ -2956,7 +3024,7 @@
       </c>
     </row>
     <row r="62" spans="3:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="124"/>
+      <c r="D62" s="119"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="25"/>
@@ -2992,7 +3060,7 @@
       </c>
     </row>
     <row r="63" spans="3:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="124"/>
+      <c r="D63" s="119"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="25"/>
@@ -3022,7 +3090,7 @@
       </c>
     </row>
     <row r="64" spans="3:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="119"/>
+      <c r="D64" s="114"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
@@ -3046,7 +3114,7 @@
       </c>
     </row>
     <row r="65" spans="4:19" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D65" s="117" t="s">
+      <c r="D65" s="124" t="s">
         <v>18</v>
       </c>
       <c r="E65" s="11"/>
@@ -3090,7 +3158,7 @@
       </c>
     </row>
     <row r="66" spans="4:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="117"/>
+      <c r="D66" s="124"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="12" t="s">
@@ -3124,7 +3192,7 @@
       </c>
     </row>
     <row r="67" spans="4:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="117"/>
+      <c r="D67" s="124"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
@@ -3146,7 +3214,7 @@
       </c>
     </row>
     <row r="68" spans="4:19" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D68" s="118" t="s">
+      <c r="D68" s="113" t="s">
         <v>19</v>
       </c>
       <c r="E68" s="11"/>
@@ -3190,7 +3258,7 @@
       </c>
     </row>
     <row r="69" spans="4:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D69" s="119"/>
+      <c r="D69" s="114"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="12" t="s">
@@ -3346,7 +3414,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="123" t="s">
+      <c r="D12" s="118" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="99"/>
@@ -3393,7 +3461,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D13" s="123"/>
+      <c r="D13" s="118"/>
       <c r="E13" s="101"/>
       <c r="F13" s="101"/>
       <c r="G13" s="100"/>
@@ -3434,7 +3502,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D14" s="123"/>
+      <c r="D14" s="118"/>
       <c r="E14" s="101"/>
       <c r="F14" s="101"/>
       <c r="G14" s="101"/>
@@ -3471,7 +3539,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D15" s="123"/>
+      <c r="D15" s="118"/>
       <c r="E15" s="101"/>
       <c r="F15" s="101"/>
       <c r="G15" s="101"/>
@@ -3508,7 +3576,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D16" s="123"/>
+      <c r="D16" s="118"/>
       <c r="E16" s="101"/>
       <c r="F16" s="101"/>
       <c r="G16" s="101"/>
@@ -3545,7 +3613,7 @@
       </c>
     </row>
     <row r="17" spans="4:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="123"/>
+      <c r="D17" s="118"/>
       <c r="E17" s="101"/>
       <c r="F17" s="101"/>
       <c r="G17" s="101"/>
@@ -3574,7 +3642,7 @@
       </c>
     </row>
     <row r="18" spans="4:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D18" s="123"/>
+      <c r="D18" s="118"/>
       <c r="E18" s="101"/>
       <c r="F18" s="101"/>
       <c r="G18" s="101"/>
@@ -3600,7 +3668,7 @@
       </c>
     </row>
     <row r="19" spans="4:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D19" s="123"/>
+      <c r="D19" s="118"/>
       <c r="E19" s="101"/>
       <c r="F19" s="101"/>
       <c r="G19" s="101"/>

</xml_diff>

<commit_message>
Planilha Projeto Proposta 2
planilha created
</commit_message>
<xml_diff>
--- a/Codigos/Cap8/VHDLCAP8.xlsx
+++ b/Codigos/Cap8/VHDLCAP8.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuário\Downloads\Cap8\Cap8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuário\Documents\GitHub\EEL7123\Codigos\Cap8\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="977" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="977"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -830,21 +830,6 @@
   </cellStyleXfs>
   <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1130,6 +1115,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,1558 +1767,1558 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="1">
         <v>43739</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="C9" s="1"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="C10" s="1"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="H11" s="7"/>
+      <c r="C11" s="1"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8" t="s">
+      <c r="G12" s="2"/>
+      <c r="H12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="4">
         <v>3</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q12" s="4">
         <v>2</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R12" s="4">
         <v>1</v>
       </c>
-      <c r="S12" s="9">
+      <c r="S12" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="6"/>
+      <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="10">
+      <c r="G13" s="2"/>
+      <c r="H13" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="5">
         <v>0</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="5">
         <v>0</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="5">
         <v>0</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="5">
         <f>36*H13+44*I13+164*J13+548*K13+36</f>
         <v>72</v>
       </c>
-      <c r="M13" s="10" t="str">
+      <c r="M13" s="5" t="str">
         <f>DEC2BIN(INT(L13/512))&amp;DEC2BIN(MOD(L13,512),9)</f>
         <v>0001001000</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="O13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P13" s="11" t="s">
+      <c r="P13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q13" s="11" t="s">
+      <c r="Q13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="R13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="S13" s="11" t="s">
+      <c r="S13" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="6"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="O14" s="9" t="s">
+      <c r="C14" s="1"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="O14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="P14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="Q14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="R14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="11" t="s">
+      <c r="S14" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
-      <c r="H15" s="7"/>
-      <c r="O15" s="9" t="s">
+      <c r="C15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="O15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P15" s="11" t="s">
+      <c r="P15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q15" s="11" t="s">
+      <c r="Q15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R15" s="11" t="s">
+      <c r="R15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="S15" s="11" t="s">
+      <c r="S15" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C16" s="6"/>
-      <c r="H16" s="7"/>
-      <c r="O16" s="9" t="s">
+      <c r="C16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="O16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="P16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="Q16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="R16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="S16" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C17" s="6"/>
-      <c r="H17" s="7"/>
+      <c r="C17" s="1"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="C18" s="1"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C19" s="6"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14">
+      <c r="C19" s="1"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9">
         <v>13</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="9">
         <v>12</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="9">
         <v>11</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="9">
         <v>10</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="9">
         <v>9</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="9">
         <v>8</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="9">
         <v>7</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="9">
         <v>6</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19" s="9">
         <v>5</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="9">
         <v>4</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19" s="9">
         <v>3</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19" s="9">
         <v>2</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q19" s="9">
         <v>1</v>
       </c>
-      <c r="R19" s="14">
+      <c r="R19" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C20" s="6"/>
-      <c r="D20" s="5" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11" t="s">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="11" t="s">
+      <c r="N20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P20" s="11" t="s">
+      <c r="P20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C22" s="6"/>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16" t="s">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="16" t="s">
+      <c r="K22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="16" t="s">
+      <c r="L22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="16" t="s">
+      <c r="M22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="N22" s="16" t="s">
+      <c r="N22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="16" t="s">
+      <c r="O22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="16" t="s">
+      <c r="P22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N23" s="11" t="s">
+      <c r="N23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O23" s="11" t="s">
+      <c r="O23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="6"/>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16" t="s">
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="I25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="J25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="16" t="s">
+      <c r="K25" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="16" t="s">
+      <c r="L25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="M25" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N25" s="16" t="s">
+      <c r="N25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O25" s="16" t="s">
+      <c r="O25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="P25" s="16" t="s">
+      <c r="P25" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C26" s="6"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15" t="s">
+      <c r="L26" s="10"/>
+      <c r="M26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C27" s="6"/>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16" t="s">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J27" s="16" t="s">
+      <c r="J27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K27" s="16" t="s">
+      <c r="K27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L27" s="16" t="s">
+      <c r="L27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M27" s="16" t="s">
+      <c r="M27" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N27" s="16" t="s">
+      <c r="N27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O27" s="16" t="s">
+      <c r="O27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="P27" s="16" t="s">
+      <c r="P27" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C28" s="6"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="6"/>
-      <c r="D29" s="17">
+      <c r="C29" s="1"/>
+      <c r="D29" s="12">
         <v>36</v>
       </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11">
         <v>1</v>
       </c>
-      <c r="N29" s="16">
+      <c r="N29" s="11">
         <v>0</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="11">
         <v>0</v>
       </c>
-      <c r="P29" s="16">
+      <c r="P29" s="11">
         <v>1</v>
       </c>
-      <c r="Q29" s="16">
+      <c r="Q29" s="11">
         <v>0</v>
       </c>
-      <c r="R29" s="16">
+      <c r="R29" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C30" s="6"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
+      <c r="C30" s="1"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C31" s="6"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
+      <c r="C31" s="1"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C32" s="6"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
+      <c r="C32" s="1"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C33" s="6"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
+      <c r="C33" s="1"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C34" s="6"/>
-      <c r="E34" s="20">
+      <c r="C34" s="1"/>
+      <c r="E34" s="15">
         <v>13</v>
       </c>
-      <c r="F34" s="20">
+      <c r="F34" s="15">
         <v>12</v>
       </c>
-      <c r="G34" s="20">
+      <c r="G34" s="15">
         <v>11</v>
       </c>
-      <c r="H34" s="20">
+      <c r="H34" s="15">
         <v>10</v>
       </c>
-      <c r="I34" s="20">
+      <c r="I34" s="15">
         <v>9</v>
       </c>
-      <c r="J34" s="20">
+      <c r="J34" s="15">
         <v>8</v>
       </c>
-      <c r="K34" s="20">
+      <c r="K34" s="15">
         <v>7</v>
       </c>
-      <c r="L34" s="20">
+      <c r="L34" s="15">
         <v>6</v>
       </c>
-      <c r="M34" s="20">
+      <c r="M34" s="15">
         <v>5</v>
       </c>
-      <c r="N34" s="20">
+      <c r="N34" s="15">
         <v>4</v>
       </c>
-      <c r="O34" s="20">
+      <c r="O34" s="15">
         <v>3</v>
       </c>
-      <c r="P34" s="20">
+      <c r="P34" s="15">
         <v>2</v>
       </c>
-      <c r="Q34" s="20">
+      <c r="Q34" s="15">
         <v>1</v>
       </c>
-      <c r="R34" s="20">
+      <c r="R34" s="15">
         <v>0</v>
       </c>
-      <c r="S34" s="21"/>
+      <c r="S34" s="16"/>
     </row>
     <row r="35" spans="3:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="6"/>
-      <c r="D35" s="3" t="s">
+      <c r="C35" s="1"/>
+      <c r="D35" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="22"/>
-      <c r="F35" s="23" t="s">
+      <c r="E35" s="17"/>
+      <c r="F35" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="23" t="s">
+      <c r="G35" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="H35" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="I35" s="23" t="s">
+      <c r="I35" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="J35" s="23" t="s">
+      <c r="J35" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K35" s="23" t="s">
+      <c r="K35" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L35" s="23" t="s">
+      <c r="L35" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M35" s="23" t="s">
+      <c r="M35" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="N35" s="23" t="s">
+      <c r="N35" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="O35" s="23" t="s">
+      <c r="O35" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="P35" s="23" t="s">
+      <c r="P35" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="24">
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C36" s="6"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23" t="s">
+      <c r="C36" s="1"/>
+      <c r="D36" s="119"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="I36" s="23" t="s">
+      <c r="I36" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K36" s="23" t="s">
+      <c r="K36" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="L36" s="23" t="s">
+      <c r="L36" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="M36" s="23" t="s">
+      <c r="M36" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="N36" s="23" t="s">
+      <c r="N36" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="O36" s="23" t="s">
+      <c r="O36" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="P36" s="23" t="s">
+      <c r="P36" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="24">
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="19">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="23" t="s">
+      <c r="C37" s="1"/>
+      <c r="D37" s="119"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="K37" s="23" t="s">
+      <c r="K37" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="L37" s="23" t="s">
+      <c r="L37" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M37" s="23" t="s">
+      <c r="M37" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="N37" s="23" t="s">
+      <c r="N37" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="O37" s="23" t="s">
+      <c r="O37" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="P37" s="23" t="s">
+      <c r="P37" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="25"/>
-      <c r="S37" s="24">
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="23" t="s">
+      <c r="C38" s="1"/>
+      <c r="D38" s="119"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="K38" s="23" t="s">
+      <c r="K38" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="L38" s="23" t="s">
+      <c r="L38" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="M38" s="23" t="s">
+      <c r="M38" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="N38" s="23" t="s">
+      <c r="N38" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="O38" s="23" t="s">
+      <c r="O38" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="P38" s="23" t="s">
+      <c r="P38" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="24">
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="19">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="3:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C39" s="6"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="23" t="s">
+      <c r="C39" s="1"/>
+      <c r="D39" s="119"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K39" s="23" t="s">
+      <c r="K39" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="L39" s="23" t="s">
+      <c r="L39" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="M39" s="23" t="s">
+      <c r="M39" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="N39" s="23" t="s">
+      <c r="N39" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O39" s="23" t="s">
+      <c r="O39" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="P39" s="26">
+      <c r="P39" s="21">
         <v>1</v>
       </c>
-      <c r="Q39" s="25"/>
-      <c r="R39" s="25"/>
-      <c r="S39" s="24">
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C40" s="6"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="23" t="s">
+      <c r="C40" s="1"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="N40" s="23" t="s">
+      <c r="N40" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="O40" s="23" t="s">
+      <c r="O40" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="25"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="24">
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="19">
         <v>6</v>
       </c>
     </row>
     <row r="41" spans="3:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C41" s="6"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="23" t="s">
+      <c r="C41" s="1"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N41" s="23" t="s">
+      <c r="N41" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="O41" s="23" t="s">
+      <c r="O41" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="24">
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="19">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="3:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C42" s="6"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="23">
+      <c r="C42" s="1"/>
+      <c r="D42" s="119"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="18">
         <v>1</v>
       </c>
-      <c r="N42" s="23" t="s">
+      <c r="N42" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O42" s="26"/>
-      <c r="P42" s="25"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="25"/>
-      <c r="S42" s="24">
+      <c r="O42" s="21"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="19">
         <v>8</v>
       </c>
     </row>
     <row r="43" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C43" s="6"/>
-      <c r="H43" s="7"/>
+      <c r="C43" s="1"/>
+      <c r="H43" s="2"/>
     </row>
     <row r="44" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C44" s="6"/>
-      <c r="H44" s="7"/>
+      <c r="C44" s="1"/>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C45" s="6"/>
-      <c r="H45" s="7"/>
+      <c r="C45" s="1"/>
+      <c r="H45" s="2"/>
     </row>
     <row r="46" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C46" s="6"/>
-      <c r="H46" s="7"/>
+      <c r="C46" s="1"/>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C47" s="6"/>
-      <c r="H47" s="7"/>
+      <c r="C47" s="1"/>
+      <c r="H47" s="2"/>
     </row>
     <row r="48" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C48" s="6"/>
-      <c r="H48" s="7"/>
+      <c r="C48" s="1"/>
+      <c r="H48" s="2"/>
     </row>
     <row r="49" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C49" s="6"/>
-      <c r="H49" s="7"/>
+      <c r="C49" s="1"/>
+      <c r="H49" s="2"/>
     </row>
     <row r="52" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="E52" s="14">
+      <c r="E52" s="9">
         <v>13</v>
       </c>
-      <c r="F52" s="14">
+      <c r="F52" s="9">
         <v>12</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G52" s="9">
         <v>11</v>
       </c>
-      <c r="H52" s="14">
+      <c r="H52" s="9">
         <v>10</v>
       </c>
-      <c r="I52" s="20">
+      <c r="I52" s="15">
         <v>9</v>
       </c>
-      <c r="J52" s="27">
+      <c r="J52" s="22">
         <v>8</v>
       </c>
-      <c r="K52" s="20">
+      <c r="K52" s="15">
         <v>7</v>
       </c>
-      <c r="L52" s="20">
+      <c r="L52" s="15">
         <v>6</v>
       </c>
-      <c r="M52" s="20">
+      <c r="M52" s="15">
         <v>5</v>
       </c>
-      <c r="N52" s="20">
+      <c r="N52" s="15">
         <v>4</v>
       </c>
-      <c r="O52" s="20">
+      <c r="O52" s="15">
         <v>3</v>
       </c>
-      <c r="P52" s="20">
+      <c r="P52" s="15">
         <v>2</v>
       </c>
-      <c r="Q52" s="14">
+      <c r="Q52" s="9">
         <v>1</v>
       </c>
-      <c r="R52" s="14">
+      <c r="R52" s="9">
         <v>0</v>
       </c>
-      <c r="S52" s="28"/>
-      <c r="U52" s="29" t="s">
+      <c r="S52" s="23"/>
+      <c r="U52" s="24" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" spans="3:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="115" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="G53" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="H53" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="I53" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="J53" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="K53" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="L53" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="M53" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="N53" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="O53" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="P53" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q53" s="37"/>
-      <c r="R53" s="11"/>
-      <c r="S53" s="24">
+      <c r="E53" s="6"/>
+      <c r="F53" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J53" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="K53" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="L53" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="M53" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="N53" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="O53" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="P53" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q53" s="32"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="19">
         <v>1</v>
       </c>
-      <c r="U53" s="38" t="s">
+      <c r="U53" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="54" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="2"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="I54" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="J54" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="K54" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="L54" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="M54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="N54" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="O54" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P54" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q54" s="45"/>
-      <c r="R54" s="39"/>
-      <c r="S54" s="24">
+      <c r="D54" s="115"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="J54" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="K54" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="L54" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="M54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="N54" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="O54" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P54" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q54" s="40"/>
+      <c r="R54" s="34"/>
+      <c r="S54" s="19">
         <v>2</v>
       </c>
-      <c r="U54" s="46" t="s">
+      <c r="U54" s="41" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="55" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D55" s="2"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="47"/>
-      <c r="J55" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="K55" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="L55" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="M55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="N55" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="O55" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P55" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q55" s="45"/>
-      <c r="R55" s="39"/>
-      <c r="S55" s="24">
+      <c r="D55" s="115"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="K55" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="L55" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="M55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="N55" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="O55" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P55" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q55" s="40"/>
+      <c r="R55" s="34"/>
+      <c r="S55" s="19">
         <v>3</v>
       </c>
-      <c r="U55" s="49" t="s">
+      <c r="U55" s="44" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="56" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D56" s="2"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="K56" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="L56" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="M56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="N56" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="O56" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="P56" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q56" s="45"/>
-      <c r="R56" s="39"/>
-      <c r="S56" s="24">
+      <c r="D56" s="115"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="K56" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="L56" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="M56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="N56" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="O56" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="P56" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q56" s="40"/>
+      <c r="R56" s="34"/>
+      <c r="S56" s="19">
         <v>4</v>
       </c>
-      <c r="U56" s="51" t="s">
+      <c r="U56" s="46" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="57" spans="3:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D57" s="2"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="K57" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L57" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="M57" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="N57" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="O57" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="P57" s="56">
+      <c r="D57" s="115"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="K57" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="L57" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="M57" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="N57" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="O57" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="P57" s="51">
         <v>1</v>
       </c>
-      <c r="Q57" s="45"/>
-      <c r="R57" s="39"/>
-      <c r="S57" s="24">
+      <c r="Q57" s="40"/>
+      <c r="R57" s="34"/>
+      <c r="S57" s="19">
         <v>5</v>
       </c>
-      <c r="U57" s="57" t="s">
+      <c r="U57" s="52" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="58" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D58" s="2"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="58"/>
-      <c r="K58" s="58"/>
-      <c r="L58" s="59"/>
-      <c r="M58" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="N58" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="O58" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="P58" s="63"/>
-      <c r="Q58" s="39"/>
-      <c r="R58" s="39"/>
-      <c r="S58" s="24">
+      <c r="D58" s="115"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="53"/>
+      <c r="L58" s="54"/>
+      <c r="M58" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="N58" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="O58" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="P58" s="58"/>
+      <c r="Q58" s="34"/>
+      <c r="R58" s="34"/>
+      <c r="S58" s="19">
         <v>6</v>
       </c>
-      <c r="U58" s="64" t="s">
+      <c r="U58" s="59" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="59" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D59" s="2"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="65"/>
-      <c r="M59" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="N59" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="O59" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="P59" s="45"/>
-      <c r="Q59" s="39"/>
-      <c r="R59" s="39"/>
-      <c r="S59" s="24">
+      <c r="D59" s="115"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="N59" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="O59" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="P59" s="40"/>
+      <c r="Q59" s="34"/>
+      <c r="R59" s="34"/>
+      <c r="S59" s="19">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="3:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D60" s="2"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="69"/>
-      <c r="G60" s="69"/>
-      <c r="H60" s="70"/>
-      <c r="I60" s="70"/>
-      <c r="J60" s="70"/>
-      <c r="K60" s="70"/>
-      <c r="L60" s="71"/>
-      <c r="M60" s="72">
+      <c r="D60" s="115"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="64"/>
+      <c r="H60" s="65"/>
+      <c r="I60" s="65"/>
+      <c r="J60" s="65"/>
+      <c r="K60" s="65"/>
+      <c r="L60" s="66"/>
+      <c r="M60" s="67">
         <v>1</v>
       </c>
-      <c r="N60" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="O60" s="74">
+      <c r="N60" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="O60" s="69">
         <v>0</v>
       </c>
-      <c r="P60" s="75"/>
-      <c r="Q60" s="69"/>
-      <c r="R60" s="69"/>
-      <c r="S60" s="76">
+      <c r="P60" s="70"/>
+      <c r="Q60" s="64"/>
+      <c r="R60" s="64"/>
+      <c r="S60" s="71">
         <v>8</v>
       </c>
     </row>
     <row r="61" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="E61" s="58"/>
-      <c r="F61" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="G61" s="78" t="s">
-        <v>55</v>
-      </c>
-      <c r="H61" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="I61" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="J61" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="K61" s="82" t="s">
-        <v>55</v>
-      </c>
-      <c r="L61" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="M61" s="84" t="s">
-        <v>55</v>
-      </c>
-      <c r="N61" s="85" t="s">
-        <v>55</v>
-      </c>
-      <c r="O61" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="P61" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q61" s="58"/>
-      <c r="R61" s="58"/>
-      <c r="S61" s="87">
+      <c r="E61" s="53"/>
+      <c r="F61" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="H61" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="I61" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="J61" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="K61" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="L61" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="M61" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="N61" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="O61" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="P61" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q61" s="53"/>
+      <c r="R61" s="53"/>
+      <c r="S61" s="82">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D62" s="1"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="88" t="s">
-        <v>55</v>
-      </c>
-      <c r="I62" s="89" t="s">
-        <v>55</v>
-      </c>
-      <c r="J62" s="90" t="s">
-        <v>55</v>
-      </c>
-      <c r="K62" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="L62" s="92" t="s">
-        <v>55</v>
-      </c>
-      <c r="M62" s="93" t="s">
-        <v>55</v>
-      </c>
-      <c r="N62" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="O62" s="95" t="s">
-        <v>55</v>
-      </c>
-      <c r="P62" s="39"/>
-      <c r="Q62" s="39"/>
-      <c r="R62" s="39"/>
-      <c r="S62" s="96">
+      <c r="D62" s="116"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="I62" s="84" t="s">
+        <v>55</v>
+      </c>
+      <c r="J62" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="K62" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="L62" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="M62" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="N62" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="O62" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="P62" s="34"/>
+      <c r="Q62" s="34"/>
+      <c r="R62" s="34"/>
+      <c r="S62" s="91">
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D63" s="1"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="39"/>
-      <c r="G63" s="50"/>
-      <c r="H63" s="97" t="s">
-        <v>55</v>
-      </c>
-      <c r="I63" s="98" t="s">
-        <v>55</v>
-      </c>
-      <c r="J63" s="99"/>
-      <c r="K63" s="100"/>
-      <c r="L63" s="101" t="s">
-        <v>55</v>
-      </c>
-      <c r="M63" s="102" t="s">
-        <v>55</v>
-      </c>
-      <c r="N63" s="103" t="s">
-        <v>55</v>
-      </c>
-      <c r="O63" s="45"/>
-      <c r="P63" s="39"/>
-      <c r="Q63" s="39"/>
-      <c r="R63" s="39"/>
-      <c r="S63" s="96">
+      <c r="D63" s="116"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="92" t="s">
+        <v>55</v>
+      </c>
+      <c r="I63" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="J63" s="94"/>
+      <c r="K63" s="95"/>
+      <c r="L63" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="M63" s="97" t="s">
+        <v>55</v>
+      </c>
+      <c r="N63" s="98" t="s">
+        <v>55</v>
+      </c>
+      <c r="O63" s="40"/>
+      <c r="P63" s="34"/>
+      <c r="Q63" s="34"/>
+      <c r="R63" s="34"/>
+      <c r="S63" s="91">
         <v>3</v>
       </c>
     </row>
     <row r="64" spans="3:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D64" s="1"/>
-      <c r="E64" s="69"/>
-      <c r="F64" s="69"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="104"/>
-      <c r="I64" s="104"/>
-      <c r="J64" s="69"/>
-      <c r="K64" s="69"/>
-      <c r="L64" s="105"/>
-      <c r="M64" s="106" t="s">
-        <v>55</v>
-      </c>
-      <c r="N64" s="107" t="s">
-        <v>55</v>
-      </c>
-      <c r="O64" s="69"/>
-      <c r="P64" s="69"/>
-      <c r="Q64" s="69"/>
-      <c r="R64" s="69"/>
-      <c r="S64" s="108">
+      <c r="D64" s="116"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
+      <c r="H64" s="99"/>
+      <c r="I64" s="99"/>
+      <c r="J64" s="64"/>
+      <c r="K64" s="64"/>
+      <c r="L64" s="100"/>
+      <c r="M64" s="101" t="s">
+        <v>55</v>
+      </c>
+      <c r="N64" s="102" t="s">
+        <v>55</v>
+      </c>
+      <c r="O64" s="64"/>
+      <c r="P64" s="64"/>
+      <c r="Q64" s="64"/>
+      <c r="R64" s="64"/>
+      <c r="S64" s="103">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="4:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="E65" s="58"/>
-      <c r="F65" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="G65" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="H65" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="I65" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="J65" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="K65" s="109" t="s">
-        <v>55</v>
-      </c>
-      <c r="L65" s="110" t="s">
-        <v>55</v>
-      </c>
-      <c r="M65" s="111" t="s">
-        <v>55</v>
-      </c>
-      <c r="N65" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="O65" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="P65" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q65" s="58"/>
-      <c r="R65" s="58"/>
-      <c r="S65" s="112">
+      <c r="E65" s="53"/>
+      <c r="F65" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="G65" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="H65" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="I65" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="J65" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="K65" s="104" t="s">
+        <v>55</v>
+      </c>
+      <c r="L65" s="105" t="s">
+        <v>55</v>
+      </c>
+      <c r="M65" s="106" t="s">
+        <v>55</v>
+      </c>
+      <c r="N65" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="O65" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="P65" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q65" s="53"/>
+      <c r="R65" s="53"/>
+      <c r="S65" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="4:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D66" s="1"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="H66" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="I66" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="J66" s="77"/>
-      <c r="K66" s="113"/>
-      <c r="L66" s="114" t="s">
-        <v>55</v>
-      </c>
-      <c r="M66" s="115" t="s">
-        <v>55</v>
-      </c>
-      <c r="N66" s="95" t="s">
-        <v>55</v>
-      </c>
-      <c r="O66" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="P66" s="39"/>
-      <c r="Q66" s="39"/>
-      <c r="R66" s="39"/>
-      <c r="S66" s="116">
+      <c r="D66" s="116"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="H66" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="I66" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66" s="72"/>
+      <c r="K66" s="108"/>
+      <c r="L66" s="109" t="s">
+        <v>55</v>
+      </c>
+      <c r="M66" s="110" t="s">
+        <v>55</v>
+      </c>
+      <c r="N66" s="90" t="s">
+        <v>55</v>
+      </c>
+      <c r="O66" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="P66" s="34"/>
+      <c r="Q66" s="34"/>
+      <c r="R66" s="34"/>
+      <c r="S66" s="111">
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="4:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D67" s="1"/>
-      <c r="E67" s="69"/>
-      <c r="F67" s="69"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="69"/>
-      <c r="J67" s="69"/>
-      <c r="K67" s="69"/>
-      <c r="L67" s="117"/>
-      <c r="M67" s="118" t="s">
-        <v>55</v>
-      </c>
-      <c r="N67" s="75"/>
-      <c r="O67" s="69"/>
-      <c r="P67" s="69"/>
-      <c r="Q67" s="69"/>
-      <c r="R67" s="69"/>
-      <c r="S67" s="119">
+      <c r="D67" s="116"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="64"/>
+      <c r="I67" s="64"/>
+      <c r="J67" s="64"/>
+      <c r="K67" s="64"/>
+      <c r="L67" s="112"/>
+      <c r="M67" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="N67" s="70"/>
+      <c r="O67" s="64"/>
+      <c r="P67" s="64"/>
+      <c r="Q67" s="64"/>
+      <c r="R67" s="64"/>
+      <c r="S67" s="114">
         <v>3</v>
       </c>
     </row>
     <row r="68" spans="4:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="E68" s="58"/>
-      <c r="F68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="G68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="H68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="I68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="J68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="K68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="L68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="M68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="N68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="O68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="P68" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q68" s="58"/>
-      <c r="R68" s="58"/>
-      <c r="S68" s="112">
+      <c r="E68" s="53"/>
+      <c r="F68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="G68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="I68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="J68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="K68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="L68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="M68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="N68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="O68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="P68" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q68" s="53"/>
+      <c r="R68" s="53"/>
+      <c r="S68" s="107">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="4:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D69" s="1"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
-      <c r="G69" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="H69" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="I69" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="J69" s="39"/>
-      <c r="K69" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="L69" s="39"/>
-      <c r="M69" s="39"/>
-      <c r="N69" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="O69" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="P69" s="39"/>
-      <c r="Q69" s="39"/>
-      <c r="R69" s="39"/>
-      <c r="S69" s="116">
+      <c r="D69" s="116"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="H69" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="I69" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="J69" s="34"/>
+      <c r="K69" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="L69" s="34"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="O69" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="P69" s="34"/>
+      <c r="Q69" s="34"/>
+      <c r="R69" s="34"/>
+      <c r="S69" s="111">
         <v>2</v>
       </c>
     </row>
@@ -3344,7 +3344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -3397,357 +3397,357 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="1">
         <v>43739</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E11" s="20">
+      <c r="E11" s="15">
         <v>13</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="15">
         <v>12</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="15">
         <v>11</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="15">
         <v>10</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="15">
         <v>9</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="15">
         <v>8</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="15">
         <v>7</v>
       </c>
-      <c r="L11" s="20">
+      <c r="L11" s="15">
         <v>6</v>
       </c>
-      <c r="M11" s="20">
+      <c r="M11" s="15">
         <v>5</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="15">
         <v>4</v>
       </c>
-      <c r="O11" s="20">
+      <c r="O11" s="15">
         <v>3</v>
       </c>
-      <c r="P11" s="20">
+      <c r="P11" s="15">
         <v>2</v>
       </c>
-      <c r="Q11" s="20">
+      <c r="Q11" s="15">
         <v>1</v>
       </c>
-      <c r="R11" s="20">
+      <c r="R11" s="15">
         <v>0</v>
       </c>
-      <c r="S11" s="21"/>
-      <c r="U11" s="29" t="s">
+      <c r="S11" s="16"/>
+      <c r="U11" s="24" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="O12" s="23" t="s">
+      <c r="O12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="P12" s="23" t="s">
+      <c r="P12" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="24">
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="19">
         <v>1</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="U12" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D13" s="3"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23" t="s">
+      <c r="D13" s="119"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="N13" s="23" t="s">
+      <c r="N13" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="23" t="s">
+      <c r="O13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="P13" s="23" t="s">
+      <c r="P13" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="24">
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="19">
         <v>2</v>
       </c>
-      <c r="U13" s="46" t="s">
+      <c r="U13" s="41" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D14" s="3"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23" t="s">
+      <c r="D14" s="119"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="K14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="L14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="23" t="s">
+      <c r="M14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="N14" s="23" t="s">
+      <c r="N14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="O14" s="23" t="s">
+      <c r="O14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="P14" s="23" t="s">
+      <c r="P14" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="24">
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="19">
         <v>3</v>
       </c>
-      <c r="U14" s="49" t="s">
+      <c r="U14" s="44" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D15" s="3"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="23" t="s">
+      <c r="D15" s="119"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="N15" s="23" t="s">
+      <c r="N15" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="23" t="s">
+      <c r="O15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="23" t="s">
+      <c r="P15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="24">
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="19">
         <v>4</v>
       </c>
-      <c r="U15" s="51" t="s">
+      <c r="U15" s="46" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D16" s="3"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="23" t="s">
+      <c r="D16" s="119"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="L16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="23" t="s">
+      <c r="M16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="N16" s="23" t="s">
+      <c r="N16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="P16" s="26">
+      <c r="P16" s="21">
         <v>1</v>
       </c>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="24">
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="19">
         <v>5</v>
       </c>
-      <c r="U16" s="57" t="s">
+      <c r="U16" s="52" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="4:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="3"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23" t="s">
+      <c r="D17" s="119"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="L17" s="23" t="s">
+      <c r="L17" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="N17" s="23" t="s">
+      <c r="N17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="23" t="s">
+      <c r="O17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="24">
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="19">
         <v>6</v>
       </c>
-      <c r="U17" s="64" t="s">
+      <c r="U17" s="59" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="18" spans="4:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D18" s="3"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23" t="s">
+      <c r="D18" s="119"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M18" s="23" t="s">
+      <c r="M18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N18" s="23" t="s">
+      <c r="N18" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="O18" s="23" t="s">
+      <c r="O18" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="24">
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="19">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="4:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D19" s="3"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="23" t="s">
+      <c r="D19" s="119"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="25"/>
-      <c r="M19" s="23">
+      <c r="L19" s="20"/>
+      <c r="M19" s="18">
         <v>1</v>
       </c>
-      <c r="N19" s="23" t="s">
+      <c r="N19" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="O19" s="26"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="24">
+      <c r="O19" s="21"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="19">
         <v>8</v>
       </c>
     </row>

</xml_diff>